<commit_message>
Updated Test025.xlsx, added Test027.xlsx and Test028.xlsx
</commit_message>
<xml_diff>
--- a/data/qa/QTP/Test025.xlsx
+++ b/data/qa/QTP/Test025.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Expected Result</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>If Status= Loaded, proceed to next Step; if not, then go to Step 9</t>
+  </si>
+  <si>
+    <t>In Existing Platforms table, under Platform Name colum, look for "HG-U133A" and Check for Status = Loaded</t>
   </si>
 </sst>
 </file>
@@ -468,7 +471,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -689,7 +692,7 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="H15" t="s">
         <v>26</v>

</xml_diff>